<commit_message>
check all chapt and add thanks, abstractE, personal publication
</commit_message>
<xml_diff>
--- a/毕业要求/博士毕业阶段规划.xlsx
+++ b/毕业要求/博士毕业阶段规划.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\thesis\毕业要求\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thesis\毕业要求\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>modulator 论文</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>第一章</t>
+  </si>
+  <si>
+    <t>论文初稿完成</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -388,7 +391,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +457,12 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>42462</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>